<commit_message>
Removed unnecessary addpath for subfolder
</commit_message>
<xml_diff>
--- a/2023_Panels/SIS_layup.xlsx
+++ b/2023_Panels/SIS_layup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMT\Documents\GitHub\modifiedCLT\2023_Panels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AA13A7-8F62-4C1C-AF5F-689614764DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DF99C1-5473-4EB6-AA0A-309046D05C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32325" yWindow="480" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31095" yWindow="2445" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,13 +30,13 @@
     <t>layer_no</t>
   </si>
   <si>
-    <t>material</t>
-  </si>
-  <si>
     <t>orientation</t>
   </si>
   <si>
     <t>thickness</t>
+  </si>
+  <si>
+    <t>material_id</t>
   </si>
 </sst>
 </file>
@@ -358,23 +358,29 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>